<commit_message>
major edits to crypto full course
</commit_message>
<xml_diff>
--- a/6.Crypto/1.Full Course/1.ModularArithmetic/Cryptology1-Modular-Arithmetic-SS.xlsx
+++ b/6.Crypto/1.Full Course/1.ModularArithmetic/Cryptology1-Modular-Arithmetic-SS.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\CyberSec-Modules\6.Crypto\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\CyberSec-Modules\6.Crypto\1.Full Course\1.ModularArithmetic\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9213C4CF-DC7C-465A-9C8D-263AFDA4B8AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{670FF2AC-0C12-44D8-8BB5-520F8E680F3E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{E08F4E7E-EFE7-4CF7-AB1D-E18BE1C035D3}"/>
+    <workbookView xWindow="22932" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{E08F4E7E-EFE7-4CF7-AB1D-E18BE1C035D3}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -487,7 +487,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -497,19 +497,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{104F1DE2-6BB9-4944-A1ED-22CF0E0894BF}">
   <dimension ref="A1:AA23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="AA23" sqref="AA23"/>
+    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="174" zoomScaleNormal="174" workbookViewId="0">
+      <selection activeCell="AA16" sqref="AA16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="17" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="2.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="2.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="9" width="3" bestFit="1" customWidth="1"/>
     <col min="10" max="27" width="4" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>25</v>
       </c>
@@ -617,7 +617,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:27" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>0</v>
       </c>
@@ -697,7 +697,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="3" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>27</v>
       </c>
@@ -806,7 +806,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="4" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>30</v>
       </c>
@@ -915,7 +915,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="5" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:27" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>0</v>
       </c>
@@ -995,7 +995,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="7" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>28</v>
       </c>
@@ -1104,7 +1104,7 @@
         <v>325</v>
       </c>
     </row>
-    <row r="8" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>29</v>
       </c>
@@ -1213,7 +1213,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="9" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:27" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>0</v>
       </c>
@@ -1293,7 +1293,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="12" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>25</v>
       </c>
@@ -1401,7 +1401,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="13" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:27" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
         <v>0</v>
       </c>
@@ -1481,7 +1481,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="14" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>26</v>
       </c>
@@ -1590,7 +1590,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="15" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>32</v>
       </c>
@@ -1699,7 +1699,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="16" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:27" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
         <v>0</v>
       </c>
@@ -1719,7 +1719,7 @@
         <v>14</v>
       </c>
       <c r="H16" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="I16" t="s">
         <v>20</v>
@@ -1746,7 +1746,7 @@
         <v>15</v>
       </c>
       <c r="Q16" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="R16" t="s">
         <v>21</v>
@@ -1767,7 +1767,7 @@
         <v>11</v>
       </c>
       <c r="X16" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="Y16" t="s">
         <v>16</v>
@@ -1776,10 +1776,10 @@
         <v>19</v>
       </c>
       <c r="AA16" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
-    <row r="19" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>25</v>
       </c>
@@ -1887,7 +1887,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="20" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:27" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
         <v>0</v>
       </c>
@@ -1967,7 +1967,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="21" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>33</v>
       </c>
@@ -2076,7 +2076,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="22" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>34</v>
       </c>
@@ -2185,7 +2185,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="23" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:27" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
         <v>0</v>
       </c>

</xml_diff>